<commit_message>
Finished hierarchical and mixed effects models
</commit_message>
<xml_diff>
--- a/Statistical_Quality_Control_Montgomery_Book/data/ch08.xlsx
+++ b/Statistical_Quality_Control_Montgomery_Book/data/ch08.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qfli\DataCamp_Digest\Statistical_Quality_Control_Montgomery_Book\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11255BB8-4117-4757-B10E-34238839E186}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9B6D5E-AE51-4FB8-9392-2CBE7F65747E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exercise data" sheetId="1" r:id="rId1"/>
-    <sheet name="Ex8-2" sheetId="2" r:id="rId2"/>
-    <sheet name="Ex8-2 cht" sheetId="3" r:id="rId3"/>
-    <sheet name="table8_1" sheetId="4" r:id="rId4"/>
+    <sheet name="table8_7" sheetId="5" r:id="rId2"/>
+    <sheet name="Ex8-2" sheetId="2" r:id="rId3"/>
+    <sheet name="Ex8-2 cht" sheetId="3" r:id="rId4"/>
+    <sheet name="table8_1" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
   <si>
     <t>Tab6-3</t>
   </si>
@@ -190,6 +191,36 @@
   </si>
   <si>
     <t>values</t>
+  </si>
+  <si>
+    <t>37 38 37 41 41 40 41 42 41</t>
+  </si>
+  <si>
+    <t>42 41 43 42 42 42 43 42 43</t>
+  </si>
+  <si>
+    <t>30 31 31 31 31 31 29 30 28</t>
+  </si>
+  <si>
+    <t>42 43 42 43 43 43 42 42 42</t>
+  </si>
+  <si>
+    <t>28 30 29 29 30 29 31 29 29</t>
+  </si>
+  <si>
+    <t>42 42 43 45 45 45 44 46 45</t>
+  </si>
+  <si>
+    <t>25 26 27 28 28 30 29 27 27</t>
+  </si>
+  <si>
+    <t>40 40 40 43 42 42 43 43 41</t>
+  </si>
+  <si>
+    <t>25 25 25 27 29 28 26 26 26</t>
+  </si>
+  <si>
+    <t>35 34 34 35 35 34 35 34 35</t>
   </si>
 </sst>
 </file>
@@ -10428,10 +10459,83 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC5D819E-4B10-4DB4-A15C-51753F6C5EC5}">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="47.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B9:E36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -10897,11 +11001,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA3BDEDB-806A-444C-B0EC-DB6B0EEE50DD}">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>